<commit_message>
beide Filter jetzt mit Farbgebung, zweite Visualisierung für beide Filter hinzugefügt
</commit_message>
<xml_diff>
--- a/uebung06/A5_Filter/a5_filter.xlsx
+++ b/uebung06/A5_Filter/a5_filter.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="5">
   <si>
     <t>Original</t>
   </si>
@@ -391,7 +391,7 @@
   <dimension ref="E3:V91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+      <selection activeCell="S19" sqref="S19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -403,21 +403,25 @@
     <col min="18" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="3" spans="5:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E3" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="L3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+    </row>
+    <row r="4" spans="5:16" x14ac:dyDescent="0.25">
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-    </row>
-    <row r="5" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+    </row>
+    <row r="5" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E5" s="2">
         <v>228</v>
       </c>
@@ -435,11 +439,23 @@
       </c>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-    </row>
-    <row r="6" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="L5" s="2">
+        <v>228</v>
+      </c>
+      <c r="M5" s="2">
+        <v>187</v>
+      </c>
+      <c r="N5" s="2">
+        <v>96</v>
+      </c>
+      <c r="O5" s="2">
+        <v>46</v>
+      </c>
+      <c r="P5" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E6" s="2">
         <v>234</v>
       </c>
@@ -457,11 +473,23 @@
       </c>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-    </row>
-    <row r="7" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="L6" s="2">
+        <v>234</v>
+      </c>
+      <c r="M6" s="2">
+        <v>203</v>
+      </c>
+      <c r="N6" s="2">
+        <v>132</v>
+      </c>
+      <c r="O6" s="2">
+        <v>71</v>
+      </c>
+      <c r="P6" s="2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E7" s="2">
         <v>252</v>
       </c>
@@ -479,11 +507,23 @@
       </c>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-    </row>
-    <row r="8" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="L7" s="2">
+        <v>252</v>
+      </c>
+      <c r="M7" s="2">
+        <v>238</v>
+      </c>
+      <c r="N7" s="2">
+        <v>158</v>
+      </c>
+      <c r="O7" s="2">
+        <v>84</v>
+      </c>
+      <c r="P7" s="2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E8" s="2">
         <v>213</v>
       </c>
@@ -501,11 +541,23 @@
       </c>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-    </row>
-    <row r="9" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="L8" s="2">
+        <v>213</v>
+      </c>
+      <c r="M8" s="2">
+        <v>199</v>
+      </c>
+      <c r="N8" s="2">
+        <v>117</v>
+      </c>
+      <c r="O8" s="2">
+        <v>58</v>
+      </c>
+      <c r="P8" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E9" s="2">
         <v>207</v>
       </c>
@@ -523,11 +575,23 @@
       </c>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
-    </row>
-    <row r="10" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="L9" s="2">
+        <v>207</v>
+      </c>
+      <c r="M9" s="2">
+        <v>185</v>
+      </c>
+      <c r="N9" s="2">
+        <v>78</v>
+      </c>
+      <c r="O9" s="2">
+        <v>44</v>
+      </c>
+      <c r="P9" s="2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
@@ -538,8 +602,10 @@
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
-    </row>
-    <row r="11" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+    </row>
+    <row r="11" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
@@ -550,8 +616,10 @@
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
-    </row>
-    <row r="12" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+    </row>
+    <row r="12" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E12" s="7" t="s">
         <v>2</v>
       </c>
@@ -561,11 +629,15 @@
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
+      <c r="L12" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
-    </row>
-    <row r="13" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+    </row>
+    <row r="13" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
@@ -576,9 +648,10 @@
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
-      <c r="O13" s="2"/>
-    </row>
-    <row r="14" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+    </row>
+    <row r="14" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E14" s="2" t="s">
         <v>4</v>
       </c>
@@ -596,12 +669,23 @@
       </c>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
-      <c r="O14" s="2"/>
-    </row>
-    <row r="15" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="L14" s="2">
+        <v>228</v>
+      </c>
+      <c r="M14" s="2">
+        <v>187</v>
+      </c>
+      <c r="N14" s="2">
+        <v>96</v>
+      </c>
+      <c r="O14" s="2">
+        <v>46</v>
+      </c>
+      <c r="P14" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E15" s="2" t="s">
         <v>4</v>
       </c>
@@ -622,49 +706,100 @@
       </c>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
-      <c r="O15" s="2"/>
-    </row>
-    <row r="16" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="L15" s="2">
+        <v>234</v>
+      </c>
+      <c r="M15" s="2">
+        <f>MEDIAN(L5,M5,N5,N6,N7,M7,L7,L6)</f>
+        <v>207.5</v>
+      </c>
+      <c r="N15" s="2">
+        <f t="shared" ref="N15:O15" si="1">MEDIAN(M5,N5,O5,O6,O7,N7,M7,M6)</f>
+        <v>127</v>
+      </c>
+      <c r="O15" s="2">
+        <f t="shared" si="1"/>
+        <v>65</v>
+      </c>
+      <c r="P15" s="2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E16" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F16" s="2">
-        <f t="shared" ref="F16:H16" si="1">MEDIAN(E6,F6,G6,G7,G8,F8,E8,E7)</f>
+        <f t="shared" ref="F16:H16" si="2">MEDIAN(E6,F6,G6,G7,G8,F8,E8,E7)</f>
         <v>201</v>
       </c>
       <c r="G16" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>124.5</v>
       </c>
       <c r="H16" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>64.5</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="O16" s="2"/>
+      <c r="L16" s="2">
+        <v>252</v>
+      </c>
+      <c r="M16" s="2">
+        <f t="shared" ref="M16:O16" si="3">MEDIAN(L6,M6,N6,N7,N8,M8,L8,L7)</f>
+        <v>201</v>
+      </c>
+      <c r="N16" s="2">
+        <f t="shared" si="3"/>
+        <v>124.5</v>
+      </c>
+      <c r="O16" s="2">
+        <f t="shared" si="3"/>
+        <v>64.5</v>
+      </c>
+      <c r="P16" s="2">
+        <v>36</v>
+      </c>
     </row>
     <row r="17" spans="5:22" x14ac:dyDescent="0.25">
       <c r="E17" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F17" s="2">
-        <f t="shared" ref="F17:H17" si="2">MEDIAN(E7,F7,G7,G8,G9,F9,E9,E8)</f>
+        <f t="shared" ref="F17:H17" si="4">MEDIAN(E7,F7,G7,G8,G9,F9,E9,E8)</f>
         <v>196</v>
       </c>
       <c r="G17" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>121</v>
       </c>
       <c r="H17" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>61</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="O17" s="2"/>
+      <c r="L17" s="2">
+        <v>213</v>
+      </c>
+      <c r="M17" s="2">
+        <f t="shared" ref="M17:O17" si="5">MEDIAN(L7,M7,N7,N8,N9,M9,L9,L8)</f>
+        <v>196</v>
+      </c>
+      <c r="N17" s="2">
+        <f t="shared" si="5"/>
+        <v>121</v>
+      </c>
+      <c r="O17" s="2">
+        <f t="shared" si="5"/>
+        <v>61</v>
+      </c>
+      <c r="P17" s="2">
+        <v>20</v>
+      </c>
     </row>
     <row r="18" spans="5:22" x14ac:dyDescent="0.25">
       <c r="E18" s="2" t="s">
@@ -682,18 +817,43 @@
       <c r="I18" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="O18" s="2"/>
+      <c r="L18" s="2">
+        <v>207</v>
+      </c>
+      <c r="M18" s="2">
+        <v>185</v>
+      </c>
+      <c r="N18" s="2">
+        <v>78</v>
+      </c>
+      <c r="O18" s="2">
+        <v>44</v>
+      </c>
+      <c r="P18" s="2">
+        <v>17</v>
+      </c>
     </row>
     <row r="19" spans="5:22" x14ac:dyDescent="0.25">
       <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
     </row>
     <row r="20" spans="5:22" x14ac:dyDescent="0.25">
       <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
     </row>
     <row r="21" spans="5:22" x14ac:dyDescent="0.25">
       <c r="E21" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="L21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
+    </row>
+    <row r="22" spans="5:22" x14ac:dyDescent="0.25">
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
     </row>
     <row r="23" spans="5:22" x14ac:dyDescent="0.25">
       <c r="E23" s="2" t="s">
@@ -711,8 +871,21 @@
       <c r="I23" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="O23" s="6"/>
-      <c r="P23" s="6"/>
+      <c r="L23" s="2">
+        <v>228</v>
+      </c>
+      <c r="M23" s="2">
+        <v>187</v>
+      </c>
+      <c r="N23" s="2">
+        <v>96</v>
+      </c>
+      <c r="O23" s="2">
+        <v>46</v>
+      </c>
+      <c r="P23" s="2">
+        <v>8</v>
+      </c>
       <c r="Q23" s="6"/>
       <c r="R23" s="2"/>
       <c r="S23" s="2"/>
@@ -724,24 +897,114 @@
       <c r="E24" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="F24" s="2">
+        <f xml:space="preserve"> AVERAGE(E5:G7)</f>
+        <v>192</v>
+      </c>
+      <c r="G24" s="2">
+        <f t="shared" ref="G24:H24" si="6" xml:space="preserve"> AVERAGE(F5:H7)</f>
+        <v>135</v>
+      </c>
+      <c r="H24" s="2">
+        <f t="shared" si="6"/>
+        <v>73</v>
+      </c>
       <c r="I24" s="2" t="s">
         <v>4</v>
+      </c>
+      <c r="L24" s="2">
+        <v>234</v>
+      </c>
+      <c r="M24" s="2">
+        <f xml:space="preserve"> AVERAGE(L5:N7)</f>
+        <v>192</v>
+      </c>
+      <c r="N24" s="2">
+        <f t="shared" ref="N24:O24" si="7" xml:space="preserve"> AVERAGE(M5:O7)</f>
+        <v>135</v>
+      </c>
+      <c r="O24" s="2">
+        <f t="shared" si="7"/>
+        <v>73</v>
+      </c>
+      <c r="P24" s="2">
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="5:22" x14ac:dyDescent="0.25">
       <c r="E25" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="F25" s="2">
+        <f t="shared" ref="F25:H25" si="8" xml:space="preserve"> AVERAGE(E6:G8)</f>
+        <v>194</v>
+      </c>
+      <c r="G25" s="2">
+        <f t="shared" si="8"/>
+        <v>140</v>
+      </c>
+      <c r="H25" s="2">
+        <f t="shared" si="8"/>
+        <v>78</v>
+      </c>
       <c r="I25" s="2" t="s">
         <v>4</v>
+      </c>
+      <c r="L25" s="2">
+        <v>252</v>
+      </c>
+      <c r="M25" s="2">
+        <f t="shared" ref="M25:O25" si="9" xml:space="preserve"> AVERAGE(L6:N8)</f>
+        <v>194</v>
+      </c>
+      <c r="N25" s="2">
+        <f t="shared" si="9"/>
+        <v>140</v>
+      </c>
+      <c r="O25" s="2">
+        <f t="shared" si="9"/>
+        <v>78</v>
+      </c>
+      <c r="P25" s="2">
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="5:22" x14ac:dyDescent="0.25">
       <c r="E26" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="F26" s="2">
+        <f t="shared" ref="F26:H26" si="10" xml:space="preserve"> AVERAGE(E7:G9)</f>
+        <v>183</v>
+      </c>
+      <c r="G26" s="2">
+        <f t="shared" si="10"/>
+        <v>129</v>
+      </c>
+      <c r="H26" s="2">
+        <f t="shared" si="10"/>
+        <v>68</v>
+      </c>
       <c r="I26" s="2" t="s">
         <v>4</v>
+      </c>
+      <c r="L26" s="2">
+        <v>213</v>
+      </c>
+      <c r="M26" s="2">
+        <f t="shared" ref="M26:O26" si="11" xml:space="preserve"> AVERAGE(L7:N9)</f>
+        <v>183</v>
+      </c>
+      <c r="N26" s="2">
+        <f t="shared" si="11"/>
+        <v>129</v>
+      </c>
+      <c r="O26" s="2">
+        <f t="shared" si="11"/>
+        <v>68</v>
+      </c>
+      <c r="P26" s="2">
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="5:22" x14ac:dyDescent="0.25">
@@ -759,6 +1022,21 @@
       </c>
       <c r="I27" s="2" t="s">
         <v>4</v>
+      </c>
+      <c r="L27" s="2">
+        <v>207</v>
+      </c>
+      <c r="M27" s="2">
+        <v>185</v>
+      </c>
+      <c r="N27" s="2">
+        <v>78</v>
+      </c>
+      <c r="O27" s="2">
+        <v>44</v>
+      </c>
+      <c r="P27" s="2">
+        <v>17</v>
       </c>
     </row>
     <row r="33" spans="13:13" x14ac:dyDescent="0.25">
@@ -769,6 +1047,324 @@
       <c r="O91" s="1"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="F6:H8">
+    <cfRule type="colorScale" priority="38">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="255"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="37">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="255"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <color theme="4" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F15:H17">
+    <cfRule type="colorScale" priority="36">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="255"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <color theme="4" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F24:H26">
+    <cfRule type="colorScale" priority="35">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="255"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <color theme="4" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M15:O17">
+    <cfRule type="colorScale" priority="32">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="255"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <color theme="4" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L5:P5">
+    <cfRule type="colorScale" priority="29">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="255"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <color theme="4" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="30">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="255"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L6:P9">
+    <cfRule type="colorScale" priority="27">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="255"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <color theme="4" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="28">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="255"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M24:O26">
+    <cfRule type="colorScale" priority="25">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="255"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <color theme="4" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="26">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="255"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M14:O14">
+    <cfRule type="colorScale" priority="23">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="255"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <color theme="4" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="24">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="255"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M23:O23">
+    <cfRule type="colorScale" priority="21">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="255"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <color theme="4" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="22">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="255"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M18:O18">
+    <cfRule type="colorScale" priority="19">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="255"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <color theme="4" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="20">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="255"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M27:O27">
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="255"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <color theme="4" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="255"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L14">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="255"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <color theme="4" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="255"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L15:L18">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="255"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <color theme="4" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="255"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L23">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="255"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <color theme="4" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="255"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L24:L27">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="255"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <color theme="4" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="255"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P14">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="255"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <color theme="4" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="255"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P15:P18">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="255"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <color theme="4" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="255"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P23">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="255"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <color theme="4" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="255"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P24:P27">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="255"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <color theme="4" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="255"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
U05 A5 fertiggestellt (bedarf aber nochmal einer genauen Überprüfung)
</commit_message>
<xml_diff>
--- a/uebung06/A5_Filter/a5_filter.xlsx
+++ b/uebung06/A5_Filter/a5_filter.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="4">
   <si>
     <t>Original</t>
   </si>
@@ -36,9 +36,6 @@
   </si>
   <si>
     <t>Boxfilter</t>
-  </si>
-  <si>
-    <t>x</t>
   </si>
 </sst>
 </file>
@@ -77,7 +74,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -85,11 +82,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -108,6 +120,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -388,22 +406,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E3:V91"/>
+  <dimension ref="E3:AL91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S19" sqref="S19"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="V13" sqref="V13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="4" width="9.140625" style="3"/>
     <col min="5" max="9" width="6.7109375" style="2" customWidth="1"/>
-    <col min="10" max="14" width="8.7109375" style="2" customWidth="1"/>
+    <col min="10" max="11" width="4.7109375" style="2" customWidth="1"/>
+    <col min="12" max="14" width="6.7109375" style="2" customWidth="1"/>
+    <col min="15" max="16" width="6.7109375" customWidth="1"/>
     <col min="17" max="17" width="8.7109375" style="2" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="3"/>
+    <col min="18" max="21" width="9.140625" style="3"/>
+    <col min="22" max="38" width="6.7109375" style="3" customWidth="1"/>
+    <col min="39" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="3" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="5:38" x14ac:dyDescent="0.25">
       <c r="E3" s="1" t="s">
         <v>0</v>
       </c>
@@ -413,7 +435,7 @@
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
     </row>
-    <row r="4" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="5:38" x14ac:dyDescent="0.25">
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
@@ -421,177 +443,402 @@
       <c r="O4" s="3"/>
       <c r="P4" s="3"/>
     </row>
-    <row r="5" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E5" s="2">
+    <row r="5" spans="5:38" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E5" s="8">
         <v>228</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="8">
         <v>187</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="9">
         <v>96</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="8">
         <v>46</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="8">
         <v>8</v>
       </c>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
-      <c r="L5" s="2">
+      <c r="L5" s="8">
         <v>228</v>
       </c>
-      <c r="M5" s="2">
+      <c r="M5" s="8">
         <v>187</v>
       </c>
-      <c r="N5" s="2">
+      <c r="N5" s="8">
         <v>96</v>
       </c>
-      <c r="O5" s="2">
+      <c r="O5" s="8">
         <v>46</v>
       </c>
-      <c r="P5" s="2">
+      <c r="P5" s="8">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E6" s="2">
+      <c r="V5" s="8">
+        <v>228</v>
+      </c>
+      <c r="W5" s="8">
+        <v>187</v>
+      </c>
+      <c r="X5" s="9">
+        <v>96</v>
+      </c>
+      <c r="Y5" s="8">
+        <v>46</v>
+      </c>
+      <c r="Z5" s="8">
+        <v>8</v>
+      </c>
+      <c r="AB5" s="8">
+        <v>228</v>
+      </c>
+      <c r="AC5" s="8">
+        <v>187</v>
+      </c>
+      <c r="AD5" s="9">
+        <v>96</v>
+      </c>
+      <c r="AE5" s="8">
+        <v>46</v>
+      </c>
+      <c r="AF5" s="8">
+        <v>8</v>
+      </c>
+      <c r="AH5" s="8">
+        <v>228</v>
+      </c>
+      <c r="AI5" s="8">
+        <v>187</v>
+      </c>
+      <c r="AJ5" s="9">
+        <v>96</v>
+      </c>
+      <c r="AK5" s="8">
+        <v>46</v>
+      </c>
+      <c r="AL5" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="5:38" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E6" s="8">
         <v>234</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="8">
         <v>203</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="9">
         <v>132</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="8">
         <v>71</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6" s="8">
         <v>26</v>
       </c>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
-      <c r="L6" s="2">
+      <c r="L6" s="8">
         <v>234</v>
       </c>
-      <c r="M6" s="2">
+      <c r="M6" s="8">
         <v>203</v>
       </c>
-      <c r="N6" s="2">
+      <c r="N6" s="8">
         <v>132</v>
       </c>
-      <c r="O6" s="2">
+      <c r="O6" s="8">
         <v>71</v>
       </c>
-      <c r="P6" s="2">
+      <c r="P6" s="8">
         <v>26</v>
       </c>
-    </row>
-    <row r="7" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E7" s="2">
+      <c r="V6" s="8">
+        <v>234</v>
+      </c>
+      <c r="W6" s="8">
+        <v>203</v>
+      </c>
+      <c r="X6" s="9">
+        <v>132</v>
+      </c>
+      <c r="Y6" s="8">
+        <v>71</v>
+      </c>
+      <c r="Z6" s="8">
+        <v>26</v>
+      </c>
+      <c r="AB6" s="8">
+        <v>234</v>
+      </c>
+      <c r="AC6" s="8">
+        <v>207.5</v>
+      </c>
+      <c r="AD6" s="8">
+        <v>127</v>
+      </c>
+      <c r="AE6" s="8">
+        <v>65</v>
+      </c>
+      <c r="AF6" s="8">
+        <v>26</v>
+      </c>
+      <c r="AH6" s="8">
+        <v>234</v>
+      </c>
+      <c r="AI6" s="8">
+        <v>192</v>
+      </c>
+      <c r="AJ6" s="8">
+        <v>135</v>
+      </c>
+      <c r="AK6" s="8">
+        <v>73</v>
+      </c>
+      <c r="AL6" s="8">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="5:38" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E7" s="8">
         <v>252</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="8">
         <v>238</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="9">
         <v>158</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="8">
         <v>84</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="8">
         <v>36</v>
       </c>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
-      <c r="L7" s="2">
+      <c r="L7" s="8">
         <v>252</v>
       </c>
-      <c r="M7" s="2">
+      <c r="M7" s="8">
         <v>238</v>
       </c>
-      <c r="N7" s="2">
+      <c r="N7" s="8">
         <v>158</v>
       </c>
-      <c r="O7" s="2">
+      <c r="O7" s="8">
         <v>84</v>
       </c>
-      <c r="P7" s="2">
+      <c r="P7" s="8">
         <v>36</v>
       </c>
-    </row>
-    <row r="8" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E8" s="2">
+      <c r="V7" s="8">
+        <v>252</v>
+      </c>
+      <c r="W7" s="8">
+        <v>238</v>
+      </c>
+      <c r="X7" s="9">
+        <v>158</v>
+      </c>
+      <c r="Y7" s="8">
+        <v>84</v>
+      </c>
+      <c r="Z7" s="8">
+        <v>36</v>
+      </c>
+      <c r="AB7" s="8">
+        <v>252</v>
+      </c>
+      <c r="AC7" s="8">
+        <v>201</v>
+      </c>
+      <c r="AD7" s="8">
+        <v>124.5</v>
+      </c>
+      <c r="AE7" s="8">
+        <v>64.5</v>
+      </c>
+      <c r="AF7" s="8">
+        <v>36</v>
+      </c>
+      <c r="AH7" s="8">
+        <v>252</v>
+      </c>
+      <c r="AI7" s="8">
+        <v>194</v>
+      </c>
+      <c r="AJ7" s="8">
+        <v>140</v>
+      </c>
+      <c r="AK7" s="8">
+        <v>78</v>
+      </c>
+      <c r="AL7" s="8">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="5:38" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E8" s="8">
         <v>213</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="8">
         <v>199</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="9">
         <v>117</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8" s="8">
         <v>58</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I8" s="8">
         <v>20</v>
       </c>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
-      <c r="L8" s="2">
+      <c r="L8" s="8">
         <v>213</v>
       </c>
-      <c r="M8" s="2">
+      <c r="M8" s="8">
         <v>199</v>
       </c>
-      <c r="N8" s="2">
+      <c r="N8" s="8">
         <v>117</v>
       </c>
-      <c r="O8" s="2">
+      <c r="O8" s="8">
         <v>58</v>
       </c>
-      <c r="P8" s="2">
+      <c r="P8" s="8">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E9" s="2">
+      <c r="V8" s="8">
+        <v>213</v>
+      </c>
+      <c r="W8" s="8">
+        <v>199</v>
+      </c>
+      <c r="X8" s="9">
+        <v>117</v>
+      </c>
+      <c r="Y8" s="8">
+        <v>58</v>
+      </c>
+      <c r="Z8" s="8">
+        <v>20</v>
+      </c>
+      <c r="AB8" s="8">
+        <v>213</v>
+      </c>
+      <c r="AC8" s="8">
+        <v>196</v>
+      </c>
+      <c r="AD8" s="8">
+        <v>121</v>
+      </c>
+      <c r="AE8" s="8">
+        <v>61</v>
+      </c>
+      <c r="AF8" s="8">
+        <v>20</v>
+      </c>
+      <c r="AH8" s="8">
+        <v>213</v>
+      </c>
+      <c r="AI8" s="8">
+        <v>183</v>
+      </c>
+      <c r="AJ8" s="8">
+        <v>129</v>
+      </c>
+      <c r="AK8" s="8">
+        <v>68</v>
+      </c>
+      <c r="AL8" s="8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="5:38" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E9" s="8">
         <v>207</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="9">
         <v>185</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="9">
         <v>78</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9" s="8">
         <v>44</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I9" s="8">
         <v>17</v>
       </c>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
-      <c r="L9" s="2">
+      <c r="L9" s="8">
         <v>207</v>
       </c>
-      <c r="M9" s="2">
+      <c r="M9" s="8">
         <v>185</v>
       </c>
-      <c r="N9" s="2">
+      <c r="N9" s="8">
         <v>78</v>
       </c>
-      <c r="O9" s="2">
+      <c r="O9" s="8">
         <v>44</v>
       </c>
-      <c r="P9" s="2">
+      <c r="P9" s="8">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="V9" s="8">
+        <v>207</v>
+      </c>
+      <c r="W9" s="9">
+        <v>185</v>
+      </c>
+      <c r="X9" s="9">
+        <v>78</v>
+      </c>
+      <c r="Y9" s="8">
+        <v>44</v>
+      </c>
+      <c r="Z9" s="8">
+        <v>17</v>
+      </c>
+      <c r="AB9" s="8">
+        <v>207</v>
+      </c>
+      <c r="AC9" s="9">
+        <v>185</v>
+      </c>
+      <c r="AD9" s="9">
+        <v>78</v>
+      </c>
+      <c r="AE9" s="8">
+        <v>44</v>
+      </c>
+      <c r="AF9" s="8">
+        <v>17</v>
+      </c>
+      <c r="AH9" s="8">
+        <v>207</v>
+      </c>
+      <c r="AI9" s="9">
+        <v>185</v>
+      </c>
+      <c r="AJ9" s="9">
+        <v>78</v>
+      </c>
+      <c r="AK9" s="8">
+        <v>44</v>
+      </c>
+      <c r="AL9" s="8">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="5:38" x14ac:dyDescent="0.25">
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
@@ -604,8 +851,17 @@
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
       <c r="P10" s="3"/>
-    </row>
-    <row r="11" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="V10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH10" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="5:38" x14ac:dyDescent="0.25">
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
@@ -619,7 +875,7 @@
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
     </row>
-    <row r="12" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="5:38" x14ac:dyDescent="0.25">
       <c r="E12" s="7" t="s">
         <v>2</v>
       </c>
@@ -637,7 +893,7 @@
       <c r="O12" s="3"/>
       <c r="P12" s="3"/>
     </row>
-    <row r="13" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="5:38" x14ac:dyDescent="0.25">
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
@@ -651,185 +907,185 @@
       <c r="O13" s="3"/>
       <c r="P13" s="3"/>
     </row>
-    <row r="14" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E14" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>4</v>
+    <row r="14" spans="5:38" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E14" s="8">
+        <v>228</v>
+      </c>
+      <c r="F14" s="8">
+        <v>187</v>
+      </c>
+      <c r="G14" s="9">
+        <v>96</v>
+      </c>
+      <c r="H14" s="8">
+        <v>46</v>
+      </c>
+      <c r="I14" s="8">
+        <v>8</v>
       </c>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
-      <c r="L14" s="2">
+      <c r="L14" s="8">
         <v>228</v>
       </c>
-      <c r="M14" s="2">
+      <c r="M14" s="8">
         <v>187</v>
       </c>
-      <c r="N14" s="2">
+      <c r="N14" s="8">
         <v>96</v>
       </c>
-      <c r="O14" s="2">
+      <c r="O14" s="8">
         <v>46</v>
       </c>
-      <c r="P14" s="2">
+      <c r="P14" s="8">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E15" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F15" s="2">
+    <row r="15" spans="5:38" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E15" s="8">
+        <v>234</v>
+      </c>
+      <c r="F15" s="8">
         <f>MEDIAN(E5,F5,G5,G6,G7,F7,E7,E6)</f>
         <v>207.5</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G15" s="8">
         <f t="shared" ref="G15:H15" si="0">MEDIAN(F5,G5,H5,H6,H7,G7,F7,F6)</f>
         <v>127</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H15" s="8">
         <f t="shared" si="0"/>
         <v>65</v>
       </c>
-      <c r="I15" s="2" t="s">
-        <v>4</v>
+      <c r="I15" s="8">
+        <v>26</v>
       </c>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
-      <c r="L15" s="2">
+      <c r="L15" s="8">
         <v>234</v>
       </c>
-      <c r="M15" s="2">
+      <c r="M15" s="8">
         <f>MEDIAN(L5,M5,N5,N6,N7,M7,L7,L6)</f>
         <v>207.5</v>
       </c>
-      <c r="N15" s="2">
+      <c r="N15" s="8">
         <f t="shared" ref="N15:O15" si="1">MEDIAN(M5,N5,O5,O6,O7,N7,M7,M6)</f>
         <v>127</v>
       </c>
-      <c r="O15" s="2">
+      <c r="O15" s="8">
         <f t="shared" si="1"/>
         <v>65</v>
       </c>
-      <c r="P15" s="2">
+      <c r="P15" s="8">
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E16" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F16" s="2">
+    <row r="16" spans="5:38" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E16" s="8">
+        <v>252</v>
+      </c>
+      <c r="F16" s="8">
         <f t="shared" ref="F16:H16" si="2">MEDIAN(E6,F6,G6,G7,G8,F8,E8,E7)</f>
         <v>201</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G16" s="8">
         <f t="shared" si="2"/>
         <v>124.5</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H16" s="8">
         <f t="shared" si="2"/>
         <v>64.5</v>
       </c>
-      <c r="I16" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L16" s="2">
+      <c r="I16" s="8">
+        <v>36</v>
+      </c>
+      <c r="L16" s="8">
         <v>252</v>
       </c>
-      <c r="M16" s="2">
+      <c r="M16" s="8">
         <f t="shared" ref="M16:O16" si="3">MEDIAN(L6,M6,N6,N7,N8,M8,L8,L7)</f>
         <v>201</v>
       </c>
-      <c r="N16" s="2">
+      <c r="N16" s="8">
         <f t="shared" si="3"/>
         <v>124.5</v>
       </c>
-      <c r="O16" s="2">
+      <c r="O16" s="8">
         <f t="shared" si="3"/>
         <v>64.5</v>
       </c>
-      <c r="P16" s="2">
+      <c r="P16" s="8">
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="5:22" x14ac:dyDescent="0.25">
-      <c r="E17" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F17" s="2">
+    <row r="17" spans="5:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E17" s="8">
+        <v>213</v>
+      </c>
+      <c r="F17" s="8">
         <f t="shared" ref="F17:H17" si="4">MEDIAN(E7,F7,G7,G8,G9,F9,E9,E8)</f>
         <v>196</v>
       </c>
-      <c r="G17" s="2">
+      <c r="G17" s="8">
         <f t="shared" si="4"/>
         <v>121</v>
       </c>
-      <c r="H17" s="2">
+      <c r="H17" s="8">
         <f t="shared" si="4"/>
         <v>61</v>
       </c>
-      <c r="I17" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L17" s="2">
+      <c r="I17" s="8">
+        <v>20</v>
+      </c>
+      <c r="L17" s="8">
         <v>213</v>
       </c>
-      <c r="M17" s="2">
+      <c r="M17" s="8">
         <f t="shared" ref="M17:O17" si="5">MEDIAN(L7,M7,N7,N8,N9,M9,L9,L8)</f>
         <v>196</v>
       </c>
-      <c r="N17" s="2">
+      <c r="N17" s="8">
         <f t="shared" si="5"/>
         <v>121</v>
       </c>
-      <c r="O17" s="2">
+      <c r="O17" s="8">
         <f t="shared" si="5"/>
         <v>61</v>
       </c>
-      <c r="P17" s="2">
+      <c r="P17" s="8">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="5:22" x14ac:dyDescent="0.25">
-      <c r="E18" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L18" s="2">
+    <row r="18" spans="5:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E18" s="8">
         <v>207</v>
       </c>
-      <c r="M18" s="2">
+      <c r="F18" s="9">
         <v>185</v>
       </c>
-      <c r="N18" s="2">
+      <c r="G18" s="9">
         <v>78</v>
       </c>
-      <c r="O18" s="2">
+      <c r="H18" s="8">
         <v>44</v>
       </c>
-      <c r="P18" s="2">
+      <c r="I18" s="8">
+        <v>17</v>
+      </c>
+      <c r="L18" s="8">
+        <v>207</v>
+      </c>
+      <c r="M18" s="8">
+        <v>185</v>
+      </c>
+      <c r="N18" s="8">
+        <v>78</v>
+      </c>
+      <c r="O18" s="8">
+        <v>44</v>
+      </c>
+      <c r="P18" s="8">
         <v>17</v>
       </c>
     </row>
@@ -855,35 +1111,35 @@
       <c r="O22" s="2"/>
       <c r="P22" s="2"/>
     </row>
-    <row r="23" spans="5:22" x14ac:dyDescent="0.25">
-      <c r="E23" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I23" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L23" s="2">
+    <row r="23" spans="5:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E23" s="8">
         <v>228</v>
       </c>
-      <c r="M23" s="2">
+      <c r="F23" s="8">
         <v>187</v>
       </c>
-      <c r="N23" s="2">
+      <c r="G23" s="9">
         <v>96</v>
       </c>
-      <c r="O23" s="2">
+      <c r="H23" s="8">
         <v>46</v>
       </c>
-      <c r="P23" s="2">
+      <c r="I23" s="8">
+        <v>8</v>
+      </c>
+      <c r="L23" s="8">
+        <v>228</v>
+      </c>
+      <c r="M23" s="8">
+        <v>187</v>
+      </c>
+      <c r="N23" s="8">
+        <v>96</v>
+      </c>
+      <c r="O23" s="8">
+        <v>46</v>
+      </c>
+      <c r="P23" s="8">
         <v>8</v>
       </c>
       <c r="Q23" s="6"/>
@@ -893,149 +1149,149 @@
       <c r="U23" s="2"/>
       <c r="V23" s="2"/>
     </row>
-    <row r="24" spans="5:22" x14ac:dyDescent="0.25">
-      <c r="E24" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F24" s="2">
+    <row r="24" spans="5:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E24" s="8">
+        <v>234</v>
+      </c>
+      <c r="F24" s="8">
         <f xml:space="preserve"> AVERAGE(E5:G7)</f>
         <v>192</v>
       </c>
-      <c r="G24" s="2">
+      <c r="G24" s="8">
         <f t="shared" ref="G24:H24" si="6" xml:space="preserve"> AVERAGE(F5:H7)</f>
         <v>135</v>
       </c>
-      <c r="H24" s="2">
+      <c r="H24" s="8">
         <f t="shared" si="6"/>
         <v>73</v>
       </c>
-      <c r="I24" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L24" s="2">
+      <c r="I24" s="8">
+        <v>26</v>
+      </c>
+      <c r="L24" s="8">
         <v>234</v>
       </c>
-      <c r="M24" s="2">
+      <c r="M24" s="8">
         <f xml:space="preserve"> AVERAGE(L5:N7)</f>
         <v>192</v>
       </c>
-      <c r="N24" s="2">
+      <c r="N24" s="8">
         <f t="shared" ref="N24:O24" si="7" xml:space="preserve"> AVERAGE(M5:O7)</f>
         <v>135</v>
       </c>
-      <c r="O24" s="2">
+      <c r="O24" s="8">
         <f t="shared" si="7"/>
         <v>73</v>
       </c>
-      <c r="P24" s="2">
+      <c r="P24" s="8">
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="5:22" x14ac:dyDescent="0.25">
-      <c r="E25" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F25" s="2">
+    <row r="25" spans="5:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E25" s="8">
+        <v>252</v>
+      </c>
+      <c r="F25" s="8">
         <f t="shared" ref="F25:H25" si="8" xml:space="preserve"> AVERAGE(E6:G8)</f>
         <v>194</v>
       </c>
-      <c r="G25" s="2">
+      <c r="G25" s="8">
         <f t="shared" si="8"/>
         <v>140</v>
       </c>
-      <c r="H25" s="2">
+      <c r="H25" s="8">
         <f t="shared" si="8"/>
         <v>78</v>
       </c>
-      <c r="I25" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L25" s="2">
+      <c r="I25" s="8">
+        <v>36</v>
+      </c>
+      <c r="L25" s="8">
         <v>252</v>
       </c>
-      <c r="M25" s="2">
+      <c r="M25" s="8">
         <f t="shared" ref="M25:O25" si="9" xml:space="preserve"> AVERAGE(L6:N8)</f>
         <v>194</v>
       </c>
-      <c r="N25" s="2">
+      <c r="N25" s="8">
         <f t="shared" si="9"/>
         <v>140</v>
       </c>
-      <c r="O25" s="2">
+      <c r="O25" s="8">
         <f t="shared" si="9"/>
         <v>78</v>
       </c>
-      <c r="P25" s="2">
+      <c r="P25" s="8">
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="5:22" x14ac:dyDescent="0.25">
-      <c r="E26" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F26" s="2">
+    <row r="26" spans="5:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E26" s="8">
+        <v>213</v>
+      </c>
+      <c r="F26" s="8">
         <f t="shared" ref="F26:H26" si="10" xml:space="preserve"> AVERAGE(E7:G9)</f>
         <v>183</v>
       </c>
-      <c r="G26" s="2">
+      <c r="G26" s="8">
         <f t="shared" si="10"/>
         <v>129</v>
       </c>
-      <c r="H26" s="2">
+      <c r="H26" s="8">
         <f t="shared" si="10"/>
         <v>68</v>
       </c>
-      <c r="I26" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L26" s="2">
+      <c r="I26" s="8">
+        <v>20</v>
+      </c>
+      <c r="L26" s="8">
         <v>213</v>
       </c>
-      <c r="M26" s="2">
+      <c r="M26" s="8">
         <f t="shared" ref="M26:O26" si="11" xml:space="preserve"> AVERAGE(L7:N9)</f>
         <v>183</v>
       </c>
-      <c r="N26" s="2">
+      <c r="N26" s="8">
         <f t="shared" si="11"/>
         <v>129</v>
       </c>
-      <c r="O26" s="2">
+      <c r="O26" s="8">
         <f t="shared" si="11"/>
         <v>68</v>
       </c>
-      <c r="P26" s="2">
+      <c r="P26" s="8">
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="5:22" x14ac:dyDescent="0.25">
-      <c r="E27" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I27" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L27" s="2">
+    <row r="27" spans="5:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E27" s="8">
         <v>207</v>
       </c>
-      <c r="M27" s="2">
+      <c r="F27" s="9">
         <v>185</v>
       </c>
-      <c r="N27" s="2">
+      <c r="G27" s="9">
         <v>78</v>
       </c>
-      <c r="O27" s="2">
+      <c r="H27" s="8">
         <v>44</v>
       </c>
-      <c r="P27" s="2">
+      <c r="I27" s="8">
+        <v>17</v>
+      </c>
+      <c r="L27" s="8">
+        <v>207</v>
+      </c>
+      <c r="M27" s="8">
+        <v>185</v>
+      </c>
+      <c r="N27" s="8">
+        <v>78</v>
+      </c>
+      <c r="O27" s="8">
+        <v>44</v>
+      </c>
+      <c r="P27" s="8">
         <v>17</v>
       </c>
     </row>
@@ -1048,7 +1304,15 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F6:H8">
-    <cfRule type="colorScale" priority="38">
+    <cfRule type="colorScale" priority="41">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="255"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <color theme="4" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="42">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="255"/>
@@ -1056,17 +1320,9 @@
         <color rgb="FFFFEF9C"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="37">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="255"/>
-        <color theme="4" tint="-0.499984740745262"/>
-        <color theme="4" tint="0.79998168889431442"/>
-      </colorScale>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F15:H17">
-    <cfRule type="colorScale" priority="36">
+    <cfRule type="colorScale" priority="40">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="255"/>
@@ -1076,35 +1332,25 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F24:H26">
-    <cfRule type="colorScale" priority="35">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="255"/>
-        <color theme="4" tint="-0.499984740745262"/>
-        <color theme="4" tint="0.79998168889431442"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M15:O17">
-    <cfRule type="colorScale" priority="32">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="255"/>
-        <color theme="4" tint="-0.499984740745262"/>
-        <color theme="4" tint="0.79998168889431442"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L5:P5">
-    <cfRule type="colorScale" priority="29">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="255"/>
-        <color theme="4" tint="-0.499984740745262"/>
-        <color theme="4" tint="0.79998168889431442"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="30">
+    <cfRule type="colorScale" priority="39">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="255"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <color theme="4" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P24:P27">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="255"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <color theme="4" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="255"/>
@@ -1113,16 +1359,26 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6:P9">
-    <cfRule type="colorScale" priority="27">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="255"/>
-        <color theme="4" tint="-0.499984740745262"/>
-        <color theme="4" tint="0.79998168889431442"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="28">
+  <conditionalFormatting sqref="M15:O17">
+    <cfRule type="colorScale" priority="36">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="255"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <color theme="4" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L5:P5">
+    <cfRule type="colorScale" priority="33">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="255"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <color theme="4" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="34">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="255"/>
@@ -1131,16 +1387,16 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M24:O26">
-    <cfRule type="colorScale" priority="25">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="255"/>
-        <color theme="4" tint="-0.499984740745262"/>
-        <color theme="4" tint="0.79998168889431442"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="26">
+  <conditionalFormatting sqref="L6:P9">
+    <cfRule type="colorScale" priority="31">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="255"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <color theme="4" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="32">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="255"/>
@@ -1149,16 +1405,16 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M14:O14">
-    <cfRule type="colorScale" priority="23">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="255"/>
-        <color theme="4" tint="-0.499984740745262"/>
-        <color theme="4" tint="0.79998168889431442"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="24">
+  <conditionalFormatting sqref="M24:O26">
+    <cfRule type="colorScale" priority="29">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="255"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <color theme="4" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="30">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="255"/>
@@ -1167,16 +1423,16 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M23:O23">
-    <cfRule type="colorScale" priority="21">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="255"/>
-        <color theme="4" tint="-0.499984740745262"/>
-        <color theme="4" tint="0.79998168889431442"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="22">
+  <conditionalFormatting sqref="M14:O14">
+    <cfRule type="colorScale" priority="27">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="255"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <color theme="4" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="28">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="255"/>
@@ -1185,16 +1441,16 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M18:O18">
-    <cfRule type="colorScale" priority="19">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="255"/>
-        <color theme="4" tint="-0.499984740745262"/>
-        <color theme="4" tint="0.79998168889431442"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="20">
+  <conditionalFormatting sqref="M23:O23">
+    <cfRule type="colorScale" priority="25">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="255"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <color theme="4" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="255"/>
@@ -1203,16 +1459,16 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M27:O27">
-    <cfRule type="colorScale" priority="17">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="255"/>
-        <color theme="4" tint="-0.499984740745262"/>
-        <color theme="4" tint="0.79998168889431442"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="18">
+  <conditionalFormatting sqref="M18:O18">
+    <cfRule type="colorScale" priority="23">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="255"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <color theme="4" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="255"/>
@@ -1221,16 +1477,16 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L14">
-    <cfRule type="colorScale" priority="15">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="255"/>
-        <color theme="4" tint="-0.499984740745262"/>
-        <color theme="4" tint="0.79998168889431442"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="16">
+  <conditionalFormatting sqref="M27:O27">
+    <cfRule type="colorScale" priority="21">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="255"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <color theme="4" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="255"/>
@@ -1239,16 +1495,16 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L15:L18">
-    <cfRule type="colorScale" priority="13">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="255"/>
-        <color theme="4" tint="-0.499984740745262"/>
-        <color theme="4" tint="0.79998168889431442"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="14">
+  <conditionalFormatting sqref="L14">
+    <cfRule type="colorScale" priority="19">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="255"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <color theme="4" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="255"/>
@@ -1257,16 +1513,16 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L23">
-    <cfRule type="colorScale" priority="11">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="255"/>
-        <color theme="4" tint="-0.499984740745262"/>
-        <color theme="4" tint="0.79998168889431442"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="12">
+  <conditionalFormatting sqref="L15:L18">
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="255"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <color theme="4" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="255"/>
@@ -1275,16 +1531,16 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L24:L27">
-    <cfRule type="colorScale" priority="9">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="255"/>
-        <color theme="4" tint="-0.499984740745262"/>
-        <color theme="4" tint="0.79998168889431442"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="10">
+  <conditionalFormatting sqref="L23">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="255"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <color theme="4" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="255"/>
@@ -1293,16 +1549,16 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P14">
-    <cfRule type="colorScale" priority="7">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="255"/>
-        <color theme="4" tint="-0.499984740745262"/>
-        <color theme="4" tint="0.79998168889431442"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="8">
+  <conditionalFormatting sqref="L24:L27">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="255"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <color theme="4" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="255"/>
@@ -1311,16 +1567,16 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P15:P18">
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="255"/>
-        <color theme="4" tint="-0.499984740745262"/>
-        <color theme="4" tint="0.79998168889431442"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="6">
+  <conditionalFormatting sqref="P14">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="255"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <color theme="4" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="255"/>
@@ -1329,16 +1585,16 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P23">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="255"/>
-        <color theme="4" tint="-0.499984740745262"/>
-        <color theme="4" tint="0.79998168889431442"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="4">
+  <conditionalFormatting sqref="P15:P18">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="255"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <color theme="4" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="255"/>
@@ -1347,21 +1603,59 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P24:P27">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="255"/>
-        <color theme="4" tint="-0.499984740745262"/>
-        <color theme="4" tint="0.79998168889431442"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="2">
+  <conditionalFormatting sqref="P23">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="255"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <color theme="4" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="255"/>
         <color rgb="FFFF7128"/>
         <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AI6:AK8">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="255"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <color theme="4" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="W6:Y8">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="255"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <color theme="4" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="255"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC6:AE8">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="255"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <color theme="4" tint="0.79998168889431442"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>

</xml_diff>